<commit_message>
Corrected comparison of strings to .equals
</commit_message>
<xml_diff>
--- a/src/main/resources/test.xlsx
+++ b/src/main/resources/test.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>R1C1</t>
   </si>
@@ -31,6 +32,9 @@
   </si>
   <si>
     <t>R4C1</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -350,7 +354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
@@ -391,4 +395,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>